<commit_message>
let binance_api_key can load from json file
</commit_message>
<xml_diff>
--- a/prediction_log/predcition_log.xlsx
+++ b/prediction_log/predcition_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1539,6 +1539,370 @@
         <v>24149.555</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2023-03-21-12:00</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>28026.1</v>
+      </c>
+      <c r="C40" t="n">
+        <v>28252.5</v>
+      </c>
+      <c r="D40" t="n">
+        <v>27907</v>
+      </c>
+      <c r="E40" t="n">
+        <v>28167.7</v>
+      </c>
+      <c r="F40" t="n">
+        <v>27941.04896359393</v>
+      </c>
+      <c r="G40" t="n">
+        <v>28119.24264361145</v>
+      </c>
+      <c r="H40" t="n">
+        <v>45890.77</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2023-03-21-13:00</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>28167.6</v>
+      </c>
+      <c r="C41" t="n">
+        <v>28200</v>
+      </c>
+      <c r="D41" t="n">
+        <v>27872.1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>28019.1</v>
+      </c>
+      <c r="F41" t="n">
+        <v>28119.24264361145</v>
+      </c>
+      <c r="G41" t="n">
+        <v>28163.20461803625</v>
+      </c>
+      <c r="H41" t="n">
+        <v>45961.945</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2023-03-21-14:00</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>28019.2</v>
+      </c>
+      <c r="C42" t="n">
+        <v>28108.5</v>
+      </c>
+      <c r="D42" t="n">
+        <v>27706</v>
+      </c>
+      <c r="E42" t="n">
+        <v>27870.5</v>
+      </c>
+      <c r="F42" t="n">
+        <v>28163.20461803625</v>
+      </c>
+      <c r="G42" t="n">
+        <v>28020.013496295</v>
+      </c>
+      <c r="H42" t="n">
+        <v>49027.562</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2023-03-21-15:00</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>27870.5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>28091.6</v>
+      </c>
+      <c r="D43" t="n">
+        <v>27838.2</v>
+      </c>
+      <c r="E43" t="n">
+        <v>28028.7</v>
+      </c>
+      <c r="F43" t="n">
+        <v>28020.013496295</v>
+      </c>
+      <c r="G43" t="n">
+        <v>28100.71539929858</v>
+      </c>
+      <c r="H43" t="n">
+        <v>25473.391</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2023-03-21-16:00</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>28028.7</v>
+      </c>
+      <c r="C44" t="n">
+        <v>28460</v>
+      </c>
+      <c r="D44" t="n">
+        <v>27998</v>
+      </c>
+      <c r="E44" t="n">
+        <v>28334.9</v>
+      </c>
+      <c r="F44" t="n">
+        <v>28100.71539929858</v>
+      </c>
+      <c r="G44" t="n">
+        <v>28273.1581835965</v>
+      </c>
+      <c r="H44" t="n">
+        <v>64811.513</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2023-03-21-17:00</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>28335</v>
+      </c>
+      <c r="C45" t="n">
+        <v>28412.4</v>
+      </c>
+      <c r="D45" t="n">
+        <v>27944</v>
+      </c>
+      <c r="E45" t="n">
+        <v>27979.9</v>
+      </c>
+      <c r="F45" t="n">
+        <v>28273.1581835965</v>
+      </c>
+      <c r="G45" t="n">
+        <v>28145.89490835118</v>
+      </c>
+      <c r="H45" t="n">
+        <v>56073.654</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2023-03-21-18:00</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>27979.8</v>
+      </c>
+      <c r="C46" t="n">
+        <v>28149</v>
+      </c>
+      <c r="D46" t="n">
+        <v>27921.5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>28119.3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>28145.89490835118</v>
+      </c>
+      <c r="G46" t="n">
+        <v>28326.42688768086</v>
+      </c>
+      <c r="H46" t="n">
+        <v>29461.273</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2023-03-21-19:00</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>28118.9</v>
+      </c>
+      <c r="C47" t="n">
+        <v>28217</v>
+      </c>
+      <c r="D47" t="n">
+        <v>28071.1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>28111.3</v>
+      </c>
+      <c r="F47" t="n">
+        <v>28326.42688768086</v>
+      </c>
+      <c r="G47" t="n">
+        <v>28178.66962040419</v>
+      </c>
+      <c r="H47" t="n">
+        <v>15047.394</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2023-03-21-20:00</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>28111.2</v>
+      </c>
+      <c r="C48" t="n">
+        <v>28200</v>
+      </c>
+      <c r="D48" t="n">
+        <v>28020</v>
+      </c>
+      <c r="E48" t="n">
+        <v>28058</v>
+      </c>
+      <c r="F48" t="n">
+        <v>28178.66962040419</v>
+      </c>
+      <c r="G48" t="n">
+        <v>28112.19943414073</v>
+      </c>
+      <c r="H48" t="n">
+        <v>14765.408</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2023-03-21-21:00</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>28058</v>
+      </c>
+      <c r="C49" t="n">
+        <v>28085</v>
+      </c>
+      <c r="D49" t="n">
+        <v>27902</v>
+      </c>
+      <c r="E49" t="n">
+        <v>27990</v>
+      </c>
+      <c r="F49" t="n">
+        <v>28112.19943414073</v>
+      </c>
+      <c r="G49" t="n">
+        <v>28094.83401953691</v>
+      </c>
+      <c r="H49" t="n">
+        <v>15159.448</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2023-03-21-22:00</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>27990</v>
+      </c>
+      <c r="C50" t="n">
+        <v>28053</v>
+      </c>
+      <c r="D50" t="n">
+        <v>27910</v>
+      </c>
+      <c r="E50" t="n">
+        <v>28019.1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>28094.83401953691</v>
+      </c>
+      <c r="G50" t="n">
+        <v>27967.14361037849</v>
+      </c>
+      <c r="H50" t="n">
+        <v>10237.152</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2023-03-21-23:00</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>28019.2</v>
+      </c>
+      <c r="C51" t="n">
+        <v>28137</v>
+      </c>
+      <c r="D51" t="n">
+        <v>27970</v>
+      </c>
+      <c r="E51" t="n">
+        <v>28091.1</v>
+      </c>
+      <c r="F51" t="n">
+        <v>27967.14361037849</v>
+      </c>
+      <c r="G51" t="n">
+        <v>28029.75347543266</v>
+      </c>
+      <c r="H51" t="n">
+        <v>10417.92</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2023-03-22-00:00</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>28091.1</v>
+      </c>
+      <c r="C52" t="n">
+        <v>28099.7</v>
+      </c>
+      <c r="D52" t="n">
+        <v>27930</v>
+      </c>
+      <c r="E52" t="n">
+        <v>28015</v>
+      </c>
+      <c r="F52" t="n">
+        <v>28029.75347543266</v>
+      </c>
+      <c r="G52" t="n">
+        <v>28088.50912627042</v>
+      </c>
+      <c r="H52" t="n">
+        <v>14113.985</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
upload a binance api key example json
</commit_message>
<xml_diff>
--- a/prediction_log/predcition_log.xlsx
+++ b/prediction_log/predcition_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1903,6 +1903,146 @@
         <v>14113.985</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2023-03-22-07:00</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>28188.9</v>
+      </c>
+      <c r="C53" t="n">
+        <v>28226.7</v>
+      </c>
+      <c r="D53" t="n">
+        <v>28002.6</v>
+      </c>
+      <c r="E53" t="n">
+        <v>28088.2</v>
+      </c>
+      <c r="F53" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="G53" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="H53" t="n">
+        <v>20732.155</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2023-03-22-07:00</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>28188.9</v>
+      </c>
+      <c r="C54" t="n">
+        <v>28226.7</v>
+      </c>
+      <c r="D54" t="n">
+        <v>28002.6</v>
+      </c>
+      <c r="E54" t="n">
+        <v>28088.2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="G54" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="H54" t="n">
+        <v>20732.155</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2023-03-22-07:00</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>28188.9</v>
+      </c>
+      <c r="C55" t="n">
+        <v>28226.7</v>
+      </c>
+      <c r="D55" t="n">
+        <v>28002.6</v>
+      </c>
+      <c r="E55" t="n">
+        <v>28088.2</v>
+      </c>
+      <c r="F55" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="G55" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="H55" t="n">
+        <v>20732.155</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2023-03-22-07:00</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>28188.9</v>
+      </c>
+      <c r="C56" t="n">
+        <v>28226.7</v>
+      </c>
+      <c r="D56" t="n">
+        <v>28002.6</v>
+      </c>
+      <c r="E56" t="n">
+        <v>28088.2</v>
+      </c>
+      <c r="F56" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="G56" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="H56" t="n">
+        <v>20732.155</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2023-03-22-08:00</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>28088.2</v>
+      </c>
+      <c r="C57" t="n">
+        <v>28213.7</v>
+      </c>
+      <c r="D57" t="n">
+        <v>28036</v>
+      </c>
+      <c r="E57" t="n">
+        <v>28071.7</v>
+      </c>
+      <c r="F57" t="n">
+        <v>28128.9540757772</v>
+      </c>
+      <c r="G57" t="n">
+        <v>28003.57721159537</v>
+      </c>
+      <c r="H57" t="n">
+        <v>18427.464</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update a easy backtesting in buy_plan v2.0.3
</commit_message>
<xml_diff>
--- a/prediction_log/predcition_log.xlsx
+++ b/prediction_log/predcition_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2043,6 +2043,146 @@
         <v>18427.464</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2023-03-22-09:00</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>28071.6</v>
+      </c>
+      <c r="C58" t="n">
+        <v>28120.7</v>
+      </c>
+      <c r="D58" t="n">
+        <v>27962.1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>28086.7</v>
+      </c>
+      <c r="F58" t="n">
+        <v>28003.57721159537</v>
+      </c>
+      <c r="G58" t="n">
+        <v>27999.57147313305</v>
+      </c>
+      <c r="H58" t="n">
+        <v>18862.109</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2023-03-22-10:00</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>28086.7</v>
+      </c>
+      <c r="C59" t="n">
+        <v>28178.6</v>
+      </c>
+      <c r="D59" t="n">
+        <v>28049.1</v>
+      </c>
+      <c r="E59" t="n">
+        <v>28138.8</v>
+      </c>
+      <c r="F59" t="n">
+        <v>27999.57147313305</v>
+      </c>
+      <c r="G59" t="n">
+        <v>28124.06128157466</v>
+      </c>
+      <c r="H59" t="n">
+        <v>13991.948</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2023-03-22-11:00</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>28138.8</v>
+      </c>
+      <c r="C60" t="n">
+        <v>28197.9</v>
+      </c>
+      <c r="D60" t="n">
+        <v>28101.8</v>
+      </c>
+      <c r="E60" t="n">
+        <v>28113.5</v>
+      </c>
+      <c r="F60" t="n">
+        <v>28124.06128157466</v>
+      </c>
+      <c r="G60" t="n">
+        <v>28099.63101356567</v>
+      </c>
+      <c r="H60" t="n">
+        <v>10376.928</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2023-03-22-12:00</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>28113.5</v>
+      </c>
+      <c r="C61" t="n">
+        <v>28241</v>
+      </c>
+      <c r="D61" t="n">
+        <v>28090.4</v>
+      </c>
+      <c r="E61" t="n">
+        <v>28207.1</v>
+      </c>
+      <c r="F61" t="n">
+        <v>28099.63101356567</v>
+      </c>
+      <c r="G61" t="n">
+        <v>28283.43265622613</v>
+      </c>
+      <c r="H61" t="n">
+        <v>19141.998</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2023-03-22-13:00</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>28207</v>
+      </c>
+      <c r="C62" t="n">
+        <v>28390</v>
+      </c>
+      <c r="D62" t="n">
+        <v>28150.5</v>
+      </c>
+      <c r="E62" t="n">
+        <v>28269.7</v>
+      </c>
+      <c r="F62" t="n">
+        <v>28283.43265622613</v>
+      </c>
+      <c r="G62" t="n">
+        <v>28399.89992704705</v>
+      </c>
+      <c r="H62" t="n">
+        <v>38841.696</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the ETH model weight for AutoPrediction
</commit_message>
<xml_diff>
--- a/prediction_log/predcition_log.xlsx
+++ b/prediction_log/predcition_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2183,6 +2183,510 @@
         <v>38841.696</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2023-03-22-14:00</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>28269.7</v>
+      </c>
+      <c r="C63" t="n">
+        <v>28758.1</v>
+      </c>
+      <c r="D63" t="n">
+        <v>28264.6</v>
+      </c>
+      <c r="E63" t="n">
+        <v>28546</v>
+      </c>
+      <c r="F63" t="n">
+        <v>28594.01502305624</v>
+      </c>
+      <c r="G63" t="n">
+        <v>28594.01502305624</v>
+      </c>
+      <c r="H63" t="n">
+        <v>97107.311</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2023-03-22-15:00</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>28545.9</v>
+      </c>
+      <c r="C64" t="n">
+        <v>28731</v>
+      </c>
+      <c r="D64" t="n">
+        <v>28423</v>
+      </c>
+      <c r="E64" t="n">
+        <v>28586.2</v>
+      </c>
+      <c r="F64" t="n">
+        <v>28594.01502305624</v>
+      </c>
+      <c r="G64" t="n">
+        <v>28670.33106257414</v>
+      </c>
+      <c r="H64" t="n">
+        <v>65870.58100000001</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2023-03-22-16:00</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>28586.1</v>
+      </c>
+      <c r="C65" t="n">
+        <v>28696.3</v>
+      </c>
+      <c r="D65" t="n">
+        <v>28469.1</v>
+      </c>
+      <c r="E65" t="n">
+        <v>28636.6</v>
+      </c>
+      <c r="F65" t="n">
+        <v>28670.33106257414</v>
+      </c>
+      <c r="G65" t="n">
+        <v>28722.41414103485</v>
+      </c>
+      <c r="H65" t="n">
+        <v>30881.951</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2023-03-22-17:00</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>28636.7</v>
+      </c>
+      <c r="C66" t="n">
+        <v>28639.1</v>
+      </c>
+      <c r="D66" t="n">
+        <v>28283.5</v>
+      </c>
+      <c r="E66" t="n">
+        <v>28500</v>
+      </c>
+      <c r="F66" t="n">
+        <v>28722.41414103485</v>
+      </c>
+      <c r="G66" t="n">
+        <v>28646.12986207716</v>
+      </c>
+      <c r="H66" t="n">
+        <v>57523.283</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2023-03-22-18:00</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>28500.4</v>
+      </c>
+      <c r="C67" t="n">
+        <v>28881</v>
+      </c>
+      <c r="D67" t="n">
+        <v>27769</v>
+      </c>
+      <c r="E67" t="n">
+        <v>28017.8</v>
+      </c>
+      <c r="F67" t="n">
+        <v>28646.12986207716</v>
+      </c>
+      <c r="G67" t="n">
+        <v>28332.9595793561</v>
+      </c>
+      <c r="H67" t="n">
+        <v>208685.849</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2023-03-22-19:00</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>28018.9</v>
+      </c>
+      <c r="C68" t="n">
+        <v>28020.3</v>
+      </c>
+      <c r="D68" t="n">
+        <v>26620</v>
+      </c>
+      <c r="E68" t="n">
+        <v>26654.1</v>
+      </c>
+      <c r="F68" t="n">
+        <v>28332.9595793561</v>
+      </c>
+      <c r="G68" t="n">
+        <v>27093.8079718299</v>
+      </c>
+      <c r="H68" t="n">
+        <v>215182.357</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2023-03-22-20:00</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>26653.3</v>
+      </c>
+      <c r="C69" t="n">
+        <v>27372</v>
+      </c>
+      <c r="D69" t="n">
+        <v>26590</v>
+      </c>
+      <c r="E69" t="n">
+        <v>27295</v>
+      </c>
+      <c r="F69" t="n">
+        <v>27093.8079718299</v>
+      </c>
+      <c r="G69" t="n">
+        <v>27421.03296262654</v>
+      </c>
+      <c r="H69" t="n">
+        <v>82764.427</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2023-03-22-21:00</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>27294.9</v>
+      </c>
+      <c r="C70" t="n">
+        <v>27425.3</v>
+      </c>
+      <c r="D70" t="n">
+        <v>27056.4</v>
+      </c>
+      <c r="E70" t="n">
+        <v>27065.3</v>
+      </c>
+      <c r="F70" t="n">
+        <v>27421.03296262654</v>
+      </c>
+      <c r="G70" t="n">
+        <v>26951.71434903986</v>
+      </c>
+      <c r="H70" t="n">
+        <v>40658.496</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2023-03-22-22:00</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>27065.3</v>
+      </c>
+      <c r="C71" t="n">
+        <v>27224</v>
+      </c>
+      <c r="D71" t="n">
+        <v>26956.3</v>
+      </c>
+      <c r="E71" t="n">
+        <v>27189.2</v>
+      </c>
+      <c r="F71" t="n">
+        <v>26951.71434903986</v>
+      </c>
+      <c r="G71" t="n">
+        <v>27108.25674876536</v>
+      </c>
+      <c r="H71" t="n">
+        <v>26901.703</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2023-03-22-23:00</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>27189.2</v>
+      </c>
+      <c r="C72" t="n">
+        <v>27333</v>
+      </c>
+      <c r="D72" t="n">
+        <v>27169.1</v>
+      </c>
+      <c r="E72" t="n">
+        <v>27233.8</v>
+      </c>
+      <c r="F72" t="n">
+        <v>27108.25674876536</v>
+      </c>
+      <c r="G72" t="n">
+        <v>27247.31263966346</v>
+      </c>
+      <c r="H72" t="n">
+        <v>18277.151</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2023-03-23-00:00</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>27233.8</v>
+      </c>
+      <c r="C73" t="n">
+        <v>27421.8</v>
+      </c>
+      <c r="D73" t="n">
+        <v>27178</v>
+      </c>
+      <c r="E73" t="n">
+        <v>27305.6</v>
+      </c>
+      <c r="F73" t="n">
+        <v>27247.31263966346</v>
+      </c>
+      <c r="G73" t="n">
+        <v>27161.47371213962</v>
+      </c>
+      <c r="H73" t="n">
+        <v>23014.289</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2023-03-23-01:00</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>27305.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>27309.2</v>
+      </c>
+      <c r="D74" t="n">
+        <v>27101</v>
+      </c>
+      <c r="E74" t="n">
+        <v>27137.9</v>
+      </c>
+      <c r="F74" t="n">
+        <v>27161.47371213962</v>
+      </c>
+      <c r="G74" t="n">
+        <v>27101.12690264694</v>
+      </c>
+      <c r="H74" t="n">
+        <v>15997.838</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2023-03-23-02:00</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>27138</v>
+      </c>
+      <c r="C75" t="n">
+        <v>27338.3</v>
+      </c>
+      <c r="D75" t="n">
+        <v>27130.5</v>
+      </c>
+      <c r="E75" t="n">
+        <v>27336.7</v>
+      </c>
+      <c r="F75" t="n">
+        <v>27101.12690264694</v>
+      </c>
+      <c r="G75" t="n">
+        <v>27214.7209693265</v>
+      </c>
+      <c r="H75" t="n">
+        <v>11407.743</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2023-03-23-03:00</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>27336.6</v>
+      </c>
+      <c r="C76" t="n">
+        <v>27415</v>
+      </c>
+      <c r="D76" t="n">
+        <v>27282.1</v>
+      </c>
+      <c r="E76" t="n">
+        <v>27343.7</v>
+      </c>
+      <c r="F76" t="n">
+        <v>27214.7209693265</v>
+      </c>
+      <c r="G76" t="n">
+        <v>27577.73025693072</v>
+      </c>
+      <c r="H76" t="n">
+        <v>13425.824</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2023-03-23-04:00</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>27343.7</v>
+      </c>
+      <c r="C77" t="n">
+        <v>27411</v>
+      </c>
+      <c r="D77" t="n">
+        <v>27231.3</v>
+      </c>
+      <c r="E77" t="n">
+        <v>27262.4</v>
+      </c>
+      <c r="F77" t="n">
+        <v>27577.73025693072</v>
+      </c>
+      <c r="G77" t="n">
+        <v>27423.21722348171</v>
+      </c>
+      <c r="H77" t="n">
+        <v>13170.433</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-03-23-05:00</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>27262.5</v>
+      </c>
+      <c r="C78" t="n">
+        <v>27680</v>
+      </c>
+      <c r="D78" t="n">
+        <v>27262.1</v>
+      </c>
+      <c r="E78" t="n">
+        <v>27608</v>
+      </c>
+      <c r="F78" t="n">
+        <v>27423.21722348171</v>
+      </c>
+      <c r="G78" t="n">
+        <v>27571.58559090094</v>
+      </c>
+      <c r="H78" t="n">
+        <v>35976.002</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2023-03-23-06:00</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>27608</v>
+      </c>
+      <c r="C79" t="n">
+        <v>27675.4</v>
+      </c>
+      <c r="D79" t="n">
+        <v>27540</v>
+      </c>
+      <c r="E79" t="n">
+        <v>27632.9</v>
+      </c>
+      <c r="F79" t="n">
+        <v>27571.58559090094</v>
+      </c>
+      <c r="G79" t="n">
+        <v>27587.91775878609</v>
+      </c>
+      <c r="H79" t="n">
+        <v>20009.877</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2023-03-23-07:00</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>27633</v>
+      </c>
+      <c r="C80" t="n">
+        <v>27660.6</v>
+      </c>
+      <c r="D80" t="n">
+        <v>27518.8</v>
+      </c>
+      <c r="E80" t="n">
+        <v>27616.4</v>
+      </c>
+      <c r="F80" t="n">
+        <v>27587.91775878609</v>
+      </c>
+      <c r="G80" t="n">
+        <v>27591.39579847406</v>
+      </c>
+      <c r="H80" t="n">
+        <v>15381.825</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>